<commit_message>
fixed some broken links and typos
</commit_message>
<xml_diff>
--- a/docs/unit1/04_flownets/flownet_calcs.xlsx
+++ b/docs/unit1/04_flownets/flownet_calcs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10102"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/My Drive (njones61@gmail.com)/work - byu/courses/CE 544/exercises/4. flow nets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/python_projects/ce544/docs/unit1/04_flownets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76C0692-1BDF-D24B-BD85-4662F9021295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C96AE17-70E9-9E4D-AD33-3D7BAB6425AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17380" yWindow="1160" windowWidth="18780" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,9 +70,6 @@
     <t>h:</t>
   </si>
   <si>
-    <t>ft/s</t>
-  </si>
-  <si>
     <t>q:</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Brigham Young University - CE 544</t>
+  </si>
+  <si>
+    <t>ft/d</t>
   </si>
 </sst>
 </file>
@@ -635,7 +635,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -656,12 +656,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -682,7 +682,7 @@
         <v>0.28346456692913385</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -705,21 +705,21 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" t="s">
@@ -728,7 +728,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" t="s">
@@ -737,21 +737,21 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -760,7 +760,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -769,7 +769,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>

</xml_diff>